<commit_message>
Updated pageLoaded for Page Classes
</commit_message>
<xml_diff>
--- a/src/test/resources/bluesource/dataProviders/TestLogin.xlsx
+++ b/src/test/resources/bluesource/dataProviders/TestLogin.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>TestScenario</t>
   </si>
@@ -31,34 +31,10 @@
     <t>COMPANY_ADMIN</t>
   </si>
   <si>
-    <t>DEPARTMENT_ADMIN</t>
-  </si>
-  <si>
-    <t>DEPARTMENT_HEAD</t>
-  </si>
-  <si>
-    <t>UPPER_MANAGEMENT</t>
-  </si>
-  <si>
-    <t>MANAGEMENT</t>
-  </si>
-  <si>
     <t>INVALID_USER</t>
   </si>
   <si>
     <t>SKIP_USER</t>
-  </si>
-  <si>
-    <t>Successful login as Management</t>
-  </si>
-  <si>
-    <t>Successful login as Upper Management</t>
-  </si>
-  <si>
-    <t>Successful login as Department Head</t>
-  </si>
-  <si>
-    <t>Successful login as Department Admin</t>
   </si>
   <si>
     <t>Successful login as Company Admin</t>
@@ -905,11 +881,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -928,42 +902,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -995,26 +937,26 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>